<commit_message>
Añadido tabla decision Contraseña y Correo
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2CD93B-D0F9-2147-AC8F-09C14E5B8A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6C8710-28F2-9945-9829-C1383764A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="116" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33:N33"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="116" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modificado casos de prueba
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6C8710-28F2-9945-9829-C1383764A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6DB503-EC71-7B4B-BD48-AB6756826959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="81">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Customer unable to click Register</t>
   </si>
   <si>
-    <t>Create an account with unexisting email but leave a required fill blank</t>
-  </si>
-  <si>
     <t>Email = guru99registered@gmail.com</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>Tester: Krivitzki, Matias</t>
+  </si>
+  <si>
+    <t>Create an account with unexisting email but a required field isn´t filled</t>
   </si>
 </sst>
 </file>
@@ -785,12 +785,54 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -799,48 +841,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1160,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
-  <dimension ref="A1:N117"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="116" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="81" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1183,10 +1183,10 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="51"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1253,16 +1253,16 @@
       <c r="E8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
+      <c r="G8" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
     </row>
     <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1277,22 +1277,22 @@
       <c r="E9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35" t="s">
+      <c r="J9" s="49"/>
+      <c r="K9" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35" t="s">
+      <c r="L9" s="49"/>
+      <c r="M9" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="N9" s="35"/>
+      <c r="N9" s="49"/>
     </row>
     <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1307,22 +1307,22 @@
       <c r="E10" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="51"/>
+      <c r="I10" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="51"/>
+      <c r="K10" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="51"/>
+      <c r="M10" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" s="37"/>
-      <c r="M10" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="N10" s="37"/>
+      <c r="N10" s="51"/>
     </row>
     <row r="11" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
@@ -1336,28 +1336,28 @@
         <v>41</v>
       </c>
       <c r="G11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="I11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="K11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="M11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" s="30" t="s">
         <v>74</v>
-      </c>
-      <c r="N11" s="30" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1368,28 +1368,28 @@
         <v>42</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L12" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N12" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.2">
@@ -1400,28 +1400,28 @@
         <v>43</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M13" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1432,28 +1432,28 @@
         <v>44</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L14" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N14" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1464,28 +1464,28 @@
         <v>45</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L15" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N15" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1496,28 +1496,28 @@
         <v>46</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K16" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L16" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N16" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1528,28 +1528,28 @@
         <v>47</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L17" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N17" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1560,156 +1560,156 @@
         <v>48</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L18" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M18" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N18" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G19" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L19" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N19" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G20" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L20" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N20" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="G21" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L21" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N21" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
       <c r="G22" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L22" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N22" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="19" t="s">
         <v>14</v>
       </c>
@@ -1717,54 +1717,54 @@
         <v>15</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L23" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N23" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G24" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N24" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1780,276 +1780,289 @@
       </c>
       <c r="E25" s="28"/>
       <c r="G25" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L25" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N25" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22">
         <v>1</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="38" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>2</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="38" t="s">
+      <c r="C27" s="34"/>
+      <c r="D27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>3</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="38" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="G28" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="N28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="G28" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>4</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="38" t="s">
+      <c r="C29" s="34"/>
+      <c r="D29" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>5</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="38" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
+      <c r="E30" s="34"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>6</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="38" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>7</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="38" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E32" s="34"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>8</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="38" t="s">
+      <c r="C33" s="34"/>
+      <c r="D33" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-    </row>
-    <row r="34" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="34"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+    </row>
+    <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>9</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="38" t="s">
+      <c r="C34" s="34"/>
+      <c r="D34" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="39"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E34" s="34"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>10</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="38" t="s">
+      <c r="C35" s="34"/>
+      <c r="D35" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="39"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>11</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="38" t="s">
+      <c r="C36" s="34"/>
+      <c r="D36" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="39"/>
-    </row>
-    <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="34"/>
+    </row>
+    <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>12</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="38" t="s">
+      <c r="C37" s="34"/>
+      <c r="D37" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="39"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E37" s="34"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>13</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="38" t="s">
+      <c r="C38" s="34"/>
+      <c r="D38" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="34"/>
+    </row>
+    <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22">
         <v>14</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="38" t="s">
+      <c r="C39" s="34"/>
+      <c r="D39" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="39"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E39" s="34"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+    </row>
+    <row r="49" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -2059,12 +2072,28 @@
       <c r="C49" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="51"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="36"/>
+      <c r="H49" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="O49" s="49"/>
+    </row>
+    <row r="50" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
@@ -2077,8 +2106,24 @@
       <c r="D50" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H50" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="51"/>
+      <c r="J50" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="K50" s="51"/>
+      <c r="L50" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="M50" s="51"/>
+      <c r="N50" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="O50" s="51"/>
+    </row>
+    <row r="51" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>4</v>
       </c>
@@ -2090,8 +2135,58 @@
       <c r="E51" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="H51" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="J51" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="K51" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="L51" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M51" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="N51" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="O51" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H52" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K52" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M52" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N52" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O52" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>6</v>
       </c>
@@ -2101,8 +2196,58 @@
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H53" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L53" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M53" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N53" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O53" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H54" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K54" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L54" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M54" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N54" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O54" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>8</v>
       </c>
@@ -2116,7 +2261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="16">
         <v>1</v>
       </c>
@@ -2127,10 +2272,10 @@
         <v>1</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="16">
         <v>2</v>
       </c>
@@ -2139,8 +2284,24 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="17"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H57" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="K57" s="47"/>
+      <c r="L57" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="M57" s="47"/>
+      <c r="N57" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="O57" s="47"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
         <v>3</v>
       </c>
@@ -2149,41 +2310,85 @@
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="17"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="48"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="48"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="16">
         <v>4</v>
       </c>
       <c r="B59" s="17"/>
       <c r="D59" s="18"/>
       <c r="E59" s="17"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="48"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="44"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="39"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="48"/>
+      <c r="N62" s="48"/>
+      <c r="O62" s="48"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="24"/>
-      <c r="B63" s="45"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="47"/>
-    </row>
-    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="B63" s="40"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="42"/>
+    </row>
+    <row r="64" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C64" s="41"/>
+      <c r="C64" s="44"/>
       <c r="D64" s="19" t="s">
         <v>14</v>
       </c>
@@ -2191,7 +2396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
         <v>16</v>
       </c>
@@ -2204,54 +2409,85 @@
       </c>
       <c r="E66" s="28"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>1</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B67" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="39"/>
-      <c r="D67" s="38" t="s">
+      <c r="C67" s="34"/>
+      <c r="D67" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="39"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E67" s="34"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="22">
         <v>2</v>
       </c>
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="38" t="s">
+      <c r="C68" s="34"/>
+      <c r="D68" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="39"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E68" s="34"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="22">
         <v>3</v>
       </c>
-      <c r="B69" s="38" t="s">
+      <c r="B69" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="39"/>
-      <c r="D69" s="38" t="s">
+      <c r="C69" s="34"/>
+      <c r="D69" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E69" s="39"/>
-    </row>
-    <row r="71" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E69" s="34"/>
+    </row>
+    <row r="71" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="29"/>
       <c r="B75" s="29"/>
       <c r="C75" s="29"/>
       <c r="D75" s="29"/>
       <c r="E75" s="29"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I79" s="49"/>
+      <c r="J79" s="49"/>
+      <c r="K79" s="49"/>
+      <c r="L79" s="49"/>
+      <c r="M79" s="49"/>
+      <c r="N79" s="49"/>
+      <c r="O79" s="49"/>
+    </row>
+    <row r="80" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I80" s="49"/>
+      <c r="J80" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="K80" s="49"/>
+      <c r="L80" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M80" s="49"/>
+      <c r="N80" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="O80" s="49"/>
+    </row>
+    <row r="81" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -2261,12 +2497,28 @@
       <c r="C81" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="E81" s="49"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D81" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" s="46"/>
+      <c r="H81" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I81" s="51"/>
+      <c r="J81" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="K81" s="51"/>
+      <c r="L81" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="M81" s="51"/>
+      <c r="N81" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="O81" s="51"/>
+    </row>
+    <row r="82" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>2</v>
       </c>
@@ -2279,8 +2531,32 @@
       <c r="D82" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H82" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I82" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="J82" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="K82" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="L82" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M82" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="N82" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="O82" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>4</v>
       </c>
@@ -2290,10 +2566,60 @@
         <v>5</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="H83" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I83" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J83" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K83" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L83" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M83" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N83" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O83" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H84" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I84" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J84" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K84" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L84" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M84" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N84" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O84" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
         <v>6</v>
       </c>
@@ -2303,8 +2629,58 @@
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H85" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I85" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J85" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K85" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L85" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M85" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N85" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O85" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H86" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I86" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J86" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K86" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L86" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M86" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N86" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O86" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>8</v>
       </c>
@@ -2317,8 +2693,32 @@
       <c r="E87" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H87" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I87" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J87" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K87" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L87" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M87" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N87" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O87" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="16">
         <v>1</v>
       </c>
@@ -2331,8 +2731,32 @@
       <c r="E88" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H88" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I88" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J88" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K88" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L88" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M88" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N88" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O88" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>2</v>
       </c>
@@ -2345,8 +2769,32 @@
       <c r="E89" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H89" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I89" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J89" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K89" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L89" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M89" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N89" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O89" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16">
         <v>3</v>
       </c>
@@ -2359,8 +2807,32 @@
       <c r="E90" s="17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H90" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I90" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J90" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K90" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L90" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M90" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N90" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O90" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>4</v>
       </c>
@@ -2371,48 +2843,192 @@
       <c r="E91" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H91" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I91" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J91" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K91" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L91" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M91" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N91" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O91" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D92" s="18">
         <v>5</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="H92" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I92" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J92" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K92" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L92" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M92" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N92" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O92" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="D93" s="18">
         <v>6</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H93" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I93" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J93" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K93" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L93" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M93" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N93" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O93" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D94" s="18">
         <v>7</v>
       </c>
       <c r="E94" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H94" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I94" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J94" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K94" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L94" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M94" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N94" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O94" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D95" s="18">
         <v>8</v>
       </c>
       <c r="E95" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H95" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I95" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J95" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K95" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L95" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M95" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N95" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O95" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D96" s="18">
         <v>9</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H96" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I96" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J96" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K96" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L96" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M96" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N96" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O96" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D97" s="18">
         <v>11</v>
       </c>
@@ -2420,40 +3036,92 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H99" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="I99" s="47"/>
+      <c r="J99" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="K99" s="47"/>
+      <c r="L99" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="M99" s="47"/>
+      <c r="N99" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="O99" s="47"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-      <c r="E100" s="44"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B100" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="39"/>
+      <c r="H100" s="48"/>
+      <c r="I100" s="48"/>
+      <c r="J100" s="48"/>
+      <c r="K100" s="48"/>
+      <c r="L100" s="48"/>
+      <c r="M100" s="48"/>
+      <c r="N100" s="48"/>
+      <c r="O100" s="48"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="24"/>
-      <c r="B101" s="45"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="46"/>
-      <c r="E101" s="47"/>
-    </row>
-    <row r="102" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="B101" s="40"/>
+      <c r="C101" s="41"/>
+      <c r="D101" s="41"/>
+      <c r="E101" s="42"/>
+      <c r="H101" s="48"/>
+      <c r="I101" s="48"/>
+      <c r="J101" s="48"/>
+      <c r="K101" s="48"/>
+      <c r="L101" s="48"/>
+      <c r="M101" s="48"/>
+      <c r="N101" s="48"/>
+      <c r="O101" s="48"/>
+    </row>
+    <row r="102" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C102" s="41"/>
+      <c r="C102" s="44"/>
       <c r="D102" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E102" s="20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H102" s="48"/>
+      <c r="I102" s="48"/>
+      <c r="J102" s="48"/>
+      <c r="K102" s="48"/>
+      <c r="L102" s="48"/>
+      <c r="M102" s="48"/>
+      <c r="N102" s="48"/>
+      <c r="O102" s="48"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H103" s="48"/>
+      <c r="I103" s="48"/>
+      <c r="J103" s="48"/>
+      <c r="K103" s="48"/>
+      <c r="L103" s="48"/>
+      <c r="M103" s="48"/>
+      <c r="N103" s="48"/>
+      <c r="O103" s="48"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="21" t="s">
         <v>16</v>
       </c>
@@ -2465,178 +3133,330 @@
         <v>18</v>
       </c>
       <c r="E104" s="28"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H104" s="48"/>
+      <c r="I104" s="48"/>
+      <c r="J104" s="48"/>
+      <c r="K104" s="48"/>
+      <c r="L104" s="48"/>
+      <c r="M104" s="48"/>
+      <c r="N104" s="48"/>
+      <c r="O104" s="48"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>1</v>
       </c>
-      <c r="B105" s="38" t="s">
+      <c r="B105" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C105" s="39"/>
-      <c r="D105" s="38" t="s">
+      <c r="C105" s="34"/>
+      <c r="D105" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E105" s="39"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E105" s="34"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
         <v>2</v>
       </c>
-      <c r="B106" s="38" t="s">
+      <c r="B106" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C106" s="39"/>
-      <c r="D106" s="38" t="s">
+      <c r="C106" s="34"/>
+      <c r="D106" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="39"/>
-    </row>
-    <row r="107" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E106" s="34"/>
+    </row>
+    <row r="107" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22">
         <v>3</v>
       </c>
-      <c r="B107" s="38" t="s">
+      <c r="B107" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="39"/>
-      <c r="D107" s="38" t="s">
+      <c r="C107" s="34"/>
+      <c r="D107" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E107" s="39"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E107" s="34"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="22">
         <v>4</v>
       </c>
-      <c r="B108" s="38" t="s">
+      <c r="B108" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C108" s="39"/>
-      <c r="D108" s="38" t="s">
+      <c r="C108" s="34"/>
+      <c r="D108" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E108" s="39"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E108" s="34"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="22">
         <v>5</v>
       </c>
-      <c r="B109" s="38" t="s">
+      <c r="B109" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C109" s="39"/>
-      <c r="D109" s="38" t="s">
+      <c r="C109" s="34"/>
+      <c r="D109" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E109" s="39"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E109" s="34"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
         <v>6</v>
       </c>
-      <c r="B110" s="38" t="s">
+      <c r="B110" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C110" s="39"/>
-      <c r="D110" s="38" t="s">
+      <c r="C110" s="34"/>
+      <c r="D110" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="39"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E110" s="34"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="22">
         <v>7</v>
       </c>
-      <c r="B111" s="38" t="s">
+      <c r="B111" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C111" s="39"/>
-      <c r="D111" s="38" t="s">
+      <c r="C111" s="34"/>
+      <c r="D111" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="39"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E111" s="34"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="22">
         <v>8</v>
       </c>
-      <c r="B112" s="38" t="s">
+      <c r="B112" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C112" s="39"/>
-      <c r="D112" s="38" t="s">
+      <c r="C112" s="34"/>
+      <c r="D112" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E112" s="39"/>
+      <c r="E112" s="34"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="22">
         <v>10</v>
       </c>
-      <c r="B113" s="38" t="s">
+      <c r="B113" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C113" s="39"/>
-      <c r="D113" s="38" t="s">
+      <c r="C113" s="34"/>
+      <c r="D113" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E113" s="39"/>
+      <c r="E113" s="34"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="22">
         <v>11</v>
       </c>
-      <c r="B114" s="38" t="s">
+      <c r="B114" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C114" s="39"/>
-      <c r="D114" s="38" t="s">
+      <c r="C114" s="34"/>
+      <c r="D114" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="39"/>
+      <c r="E114" s="34"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="22">
         <v>12</v>
       </c>
-      <c r="B115" s="38" t="s">
+      <c r="B115" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C115" s="39"/>
-      <c r="D115" s="38" t="s">
+      <c r="C115" s="34"/>
+      <c r="D115" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E115" s="39"/>
+      <c r="E115" s="34"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="22">
         <v>13</v>
       </c>
-      <c r="B116" s="38" t="s">
+      <c r="B116" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C116" s="39"/>
-      <c r="D116" s="38" t="s">
+      <c r="C116" s="34"/>
+      <c r="D116" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E116" s="39"/>
+      <c r="E116" s="34"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="22">
         <v>14</v>
       </c>
-      <c r="B117" s="38" t="s">
+      <c r="B117" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C117" s="39"/>
-      <c r="D117" s="38" t="s">
+      <c r="C117" s="34"/>
+      <c r="D117" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E117" s="39"/>
+      <c r="E117" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="168">
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="L103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:M104"/>
+    <mergeCell ref="N104:O104"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="L100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B100:E101"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B62:E63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:C28"/>
@@ -2661,84 +3481,6 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B62:E63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B100:E101"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Añadido automatizacion Caso Prueba Registrarse
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B261F815-B0A1-B742-B391-E834BB73CA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F719B-EEBE-8F40-8BA5-6C062C365A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="89">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t>Ejecutado Manualmente - ERROR - Deja registrar al usuario con el Field de City faltando. No ocurre con el field de Nombre, si Nombre falta entonces muestra advertencia de que lo complete.</t>
+  </si>
+  <si>
+    <t>No pide Fecha Nac</t>
+  </si>
+  <si>
+    <t>Pide registrar con correo existente</t>
+  </si>
+  <si>
+    <t>Deja registrar sin campo ciudad</t>
   </si>
 </sst>
 </file>
@@ -806,12 +815,60 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,54 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1189,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="81" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101:I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,10 +1219,10 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="51"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1282,16 +1291,16 @@
       <c r="E8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1306,22 +1315,22 @@
       <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35" t="s">
+      <c r="H9" s="51"/>
+      <c r="I9" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35" t="s">
+      <c r="J9" s="51"/>
+      <c r="K9" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35" t="s">
+      <c r="L9" s="51"/>
+      <c r="M9" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="35"/>
+      <c r="N9" s="51"/>
     </row>
     <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1336,22 +1345,22 @@
       <c r="E10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="36" t="s">
+      <c r="H10" s="53"/>
+      <c r="I10" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="36" t="s">
+      <c r="J10" s="53"/>
+      <c r="K10" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="37"/>
-      <c r="M10" s="36" t="s">
+      <c r="L10" s="53"/>
+      <c r="M10" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="N10" s="37"/>
+      <c r="N10" s="53"/>
     </row>
     <row r="11" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
@@ -1669,12 +1678,12 @@
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
       <c r="G21" s="31" t="s">
         <v>74</v>
       </c>
@@ -1702,10 +1711,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
       <c r="G22" s="31" t="s">
         <v>74</v>
       </c>
@@ -1735,10 +1744,10 @@
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="19" t="s">
         <v>14</v>
       </c>
@@ -1837,226 +1846,230 @@
       <c r="A26" s="22">
         <v>1</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="38" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>2</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="38" t="s">
+      <c r="C27" s="36"/>
+      <c r="D27" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="36"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>4</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="38" t="s">
+      <c r="C28" s="36"/>
+      <c r="D28" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="G28" s="34" t="s">
+      <c r="E28" s="36"/>
+      <c r="G28" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34" t="s">
+      <c r="H28" s="49"/>
+      <c r="I28" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34" t="s">
+      <c r="J28" s="49"/>
+      <c r="K28" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34" t="s">
+      <c r="L28" s="49"/>
+      <c r="M28" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="N28" s="34"/>
+      <c r="N28" s="49"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>5</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="38" t="s">
+      <c r="C29" s="36"/>
+      <c r="D29" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E29" s="36"/>
+      <c r="G29" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+    </row>
+    <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>6</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="38" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
+      <c r="E30" s="36"/>
+      <c r="G30" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>7</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="38" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
+      <c r="E31" s="36"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>8</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="38" t="s">
+      <c r="C32" s="36"/>
+      <c r="D32" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
+      <c r="E32" s="36"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>9</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="38" t="s">
+      <c r="C33" s="36"/>
+      <c r="D33" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
+      <c r="E33" s="36"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
     </row>
     <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>10</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="38" t="s">
+      <c r="C34" s="36"/>
+      <c r="D34" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="39"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>11</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="38" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="39"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>12</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="38" t="s">
+      <c r="C36" s="36"/>
+      <c r="D36" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="39"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>13</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="38" t="s">
+      <c r="C37" s="36"/>
+      <c r="D37" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="39"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>14</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="38" t="s">
+      <c r="C38" s="36"/>
+      <c r="D38" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="36"/>
     </row>
     <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2077,20 +2090,20 @@
       <c r="C48" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="50" t="s">
+      <c r="D48" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="51"/>
-      <c r="H48" s="35" t="s">
+      <c r="E48" s="38"/>
+      <c r="H48" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="35"/>
-      <c r="O48" s="35"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
+      <c r="O48" s="51"/>
     </row>
     <row r="49" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -2105,22 +2118,22 @@
       <c r="D49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="35" t="s">
+      <c r="H49" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35" t="s">
+      <c r="I49" s="51"/>
+      <c r="J49" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35" t="s">
+      <c r="K49" s="51"/>
+      <c r="L49" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35" t="s">
+      <c r="M49" s="51"/>
+      <c r="N49" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="O49" s="35"/>
+      <c r="O49" s="51"/>
     </row>
     <row r="50" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -2134,22 +2147,22 @@
       <c r="E50" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="36" t="s">
+      <c r="H50" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="37"/>
-      <c r="J50" s="36" t="s">
+      <c r="I50" s="53"/>
+      <c r="J50" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="K50" s="37"/>
-      <c r="L50" s="36" t="s">
+      <c r="K50" s="53"/>
+      <c r="L50" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="M50" s="37"/>
-      <c r="N50" s="36" t="s">
+      <c r="M50" s="53"/>
+      <c r="N50" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="O50" s="37"/>
+      <c r="O50" s="53"/>
     </row>
     <row r="51" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H51" s="30" t="s">
@@ -2253,10 +2266,10 @@
       <c r="E54" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H54" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="I54" s="53" t="s">
+      <c r="H54" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" s="34" t="s">
         <v>75</v>
       </c>
       <c r="J54" s="31" t="s">
@@ -2311,22 +2324,22 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="17"/>
-      <c r="H57" s="34" t="s">
+      <c r="H57" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="I57" s="34"/>
-      <c r="J57" s="34" t="s">
+      <c r="I57" s="49"/>
+      <c r="J57" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34" t="s">
+      <c r="K57" s="49"/>
+      <c r="L57" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="M57" s="34"/>
-      <c r="N57" s="34" t="s">
+      <c r="M57" s="49"/>
+      <c r="N57" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="34"/>
+      <c r="O57" s="49"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
@@ -2335,79 +2348,79 @@
       <c r="B58" s="17"/>
       <c r="D58" s="18"/>
       <c r="E58" s="17"/>
-      <c r="H58" s="33" t="s">
+      <c r="H58" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="33"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="50"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="50"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="50"/>
+      <c r="L59" s="50"/>
+      <c r="M59" s="50"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="50"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-      <c r="O60" s="33"/>
+      <c r="H60" s="50"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="50"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="50"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="44"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
-      <c r="O61" s="33"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="41"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="50"/>
+      <c r="M61" s="50"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="24"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="47"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="33"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="44"/>
+      <c r="H62" s="50"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="50"/>
+      <c r="K62" s="50"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="50"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="50"/>
     </row>
     <row r="63" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="41"/>
+      <c r="C63" s="46"/>
       <c r="D63" s="19" t="s">
         <v>14</v>
       </c>
@@ -2432,40 +2445,40 @@
       <c r="A66" s="22">
         <v>1</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="39"/>
-      <c r="D66" s="38" t="s">
+      <c r="C66" s="36"/>
+      <c r="D66" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="39"/>
+      <c r="E66" s="36"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>2</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B67" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="39"/>
-      <c r="D67" s="38" t="s">
+      <c r="C67" s="36"/>
+      <c r="D67" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E67" s="39"/>
+      <c r="E67" s="36"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="22">
         <v>3</v>
       </c>
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="38" t="s">
+      <c r="C68" s="36"/>
+      <c r="D68" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="39"/>
+      <c r="E68" s="36"/>
     </row>
     <row r="71" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -2477,16 +2490,16 @@
     </row>
     <row r="78" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H79" s="35" t="s">
+      <c r="H79" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I79" s="35"/>
-      <c r="J79" s="35"/>
-      <c r="K79" s="35"/>
-      <c r="L79" s="35"/>
-      <c r="M79" s="35"/>
-      <c r="N79" s="35"/>
-      <c r="O79" s="35"/>
+      <c r="I79" s="51"/>
+      <c r="J79" s="51"/>
+      <c r="K79" s="51"/>
+      <c r="L79" s="51"/>
+      <c r="M79" s="51"/>
+      <c r="N79" s="51"/>
+      <c r="O79" s="51"/>
     </row>
     <row r="80" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2498,26 +2511,26 @@
       <c r="C80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="48" t="s">
+      <c r="D80" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E80" s="49"/>
-      <c r="H80" s="35" t="s">
+      <c r="E80" s="48"/>
+      <c r="H80" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I80" s="35"/>
-      <c r="J80" s="35" t="s">
+      <c r="I80" s="51"/>
+      <c r="J80" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="K80" s="35"/>
-      <c r="L80" s="35" t="s">
+      <c r="K80" s="51"/>
+      <c r="L80" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="M80" s="35"/>
-      <c r="N80" s="35" t="s">
+      <c r="M80" s="51"/>
+      <c r="N80" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="O80" s="35"/>
+      <c r="O80" s="51"/>
     </row>
     <row r="81" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2532,22 +2545,22 @@
       <c r="D81" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H81" s="36" t="s">
+      <c r="H81" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="I81" s="37"/>
-      <c r="J81" s="36" t="s">
+      <c r="I81" s="53"/>
+      <c r="J81" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="K81" s="37"/>
-      <c r="L81" s="36" t="s">
+      <c r="K81" s="53"/>
+      <c r="L81" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="M81" s="37"/>
-      <c r="N81" s="36" t="s">
+      <c r="M81" s="53"/>
+      <c r="N81" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="O81" s="37"/>
+      <c r="O81" s="53"/>
     </row>
     <row r="82" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -3030,10 +3043,10 @@
       <c r="E96" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H96" s="52" t="s">
+      <c r="H96" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I96" s="53" t="s">
+      <c r="I96" s="34" t="s">
         <v>81</v>
       </c>
       <c r="J96" s="31" t="s">
@@ -3060,76 +3073,78 @@
       <c r="A99" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="42" t="s">
+      <c r="B99" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="43"/>
-      <c r="D99" s="43"/>
-      <c r="E99" s="44"/>
-      <c r="H99" s="34" t="s">
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="41"/>
+      <c r="H99" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="I99" s="34"/>
-      <c r="J99" s="34" t="s">
+      <c r="I99" s="49"/>
+      <c r="J99" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="K99" s="34"/>
-      <c r="L99" s="34" t="s">
+      <c r="K99" s="49"/>
+      <c r="L99" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="M99" s="34"/>
-      <c r="N99" s="34" t="s">
+      <c r="M99" s="49"/>
+      <c r="N99" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="O99" s="34"/>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O99" s="49"/>
+    </row>
+    <row r="100" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24"/>
-      <c r="B100" s="45"/>
-      <c r="C100" s="46"/>
-      <c r="D100" s="46"/>
-      <c r="E100" s="47"/>
-      <c r="H100" s="33"/>
-      <c r="I100" s="33"/>
-      <c r="J100" s="33"/>
-      <c r="K100" s="33"/>
-      <c r="L100" s="33"/>
-      <c r="M100" s="33"/>
-      <c r="N100" s="33"/>
-      <c r="O100" s="33"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+      <c r="E100" s="44"/>
+      <c r="H100" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="I100" s="50"/>
+      <c r="J100" s="50"/>
+      <c r="K100" s="50"/>
+      <c r="L100" s="50"/>
+      <c r="M100" s="50"/>
+      <c r="N100" s="50"/>
+      <c r="O100" s="50"/>
     </row>
     <row r="101" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="41"/>
+      <c r="C101" s="46"/>
       <c r="D101" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H101" s="33"/>
-      <c r="I101" s="33"/>
-      <c r="J101" s="33"/>
-      <c r="K101" s="33"/>
-      <c r="L101" s="33"/>
-      <c r="M101" s="33"/>
-      <c r="N101" s="33"/>
-      <c r="O101" s="33"/>
+      <c r="H101" s="50"/>
+      <c r="I101" s="50"/>
+      <c r="J101" s="50"/>
+      <c r="K101" s="50"/>
+      <c r="L101" s="50"/>
+      <c r="M101" s="50"/>
+      <c r="N101" s="50"/>
+      <c r="O101" s="50"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H102" s="33"/>
-      <c r="I102" s="33"/>
-      <c r="J102" s="33"/>
-      <c r="K102" s="33"/>
-      <c r="L102" s="33"/>
-      <c r="M102" s="33"/>
-      <c r="N102" s="33"/>
-      <c r="O102" s="33"/>
+      <c r="H102" s="50"/>
+      <c r="I102" s="50"/>
+      <c r="J102" s="50"/>
+      <c r="K102" s="50"/>
+      <c r="L102" s="50"/>
+      <c r="M102" s="50"/>
+      <c r="N102" s="50"/>
+      <c r="O102" s="50"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
@@ -3143,181 +3158,321 @@
         <v>18</v>
       </c>
       <c r="E103" s="28"/>
-      <c r="H103" s="33"/>
-      <c r="I103" s="33"/>
-      <c r="J103" s="33"/>
-      <c r="K103" s="33"/>
-      <c r="L103" s="33"/>
-      <c r="M103" s="33"/>
-      <c r="N103" s="33"/>
-      <c r="O103" s="33"/>
+      <c r="H103" s="50"/>
+      <c r="I103" s="50"/>
+      <c r="J103" s="50"/>
+      <c r="K103" s="50"/>
+      <c r="L103" s="50"/>
+      <c r="M103" s="50"/>
+      <c r="N103" s="50"/>
+      <c r="O103" s="50"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="22">
         <v>1</v>
       </c>
-      <c r="B104" s="38" t="s">
+      <c r="B104" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="39"/>
-      <c r="D104" s="38" t="s">
+      <c r="C104" s="36"/>
+      <c r="D104" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E104" s="39"/>
-      <c r="H104" s="33"/>
-      <c r="I104" s="33"/>
-      <c r="J104" s="33"/>
-      <c r="K104" s="33"/>
-      <c r="L104" s="33"/>
-      <c r="M104" s="33"/>
-      <c r="N104" s="33"/>
-      <c r="O104" s="33"/>
+      <c r="E104" s="36"/>
+      <c r="H104" s="50"/>
+      <c r="I104" s="50"/>
+      <c r="J104" s="50"/>
+      <c r="K104" s="50"/>
+      <c r="L104" s="50"/>
+      <c r="M104" s="50"/>
+      <c r="N104" s="50"/>
+      <c r="O104" s="50"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>2</v>
       </c>
-      <c r="B105" s="38" t="s">
+      <c r="B105" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="39"/>
-      <c r="D105" s="38" t="s">
+      <c r="C105" s="36"/>
+      <c r="D105" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="39"/>
+      <c r="E105" s="36"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
         <v>4</v>
       </c>
-      <c r="B106" s="38" t="s">
+      <c r="B106" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="39"/>
-      <c r="D106" s="38" t="s">
+      <c r="C106" s="36"/>
+      <c r="D106" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="39"/>
+      <c r="E106" s="36"/>
     </row>
     <row r="107" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22">
         <v>5</v>
       </c>
-      <c r="B107" s="38" t="s">
+      <c r="B107" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="39"/>
-      <c r="D107" s="38" t="s">
+      <c r="C107" s="36"/>
+      <c r="D107" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E107" s="39"/>
+      <c r="E107" s="36"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="22">
         <v>6</v>
       </c>
-      <c r="B108" s="38" t="s">
+      <c r="B108" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C108" s="39"/>
-      <c r="D108" s="38" t="s">
+      <c r="C108" s="36"/>
+      <c r="D108" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E108" s="39"/>
+      <c r="E108" s="36"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="22">
         <v>7</v>
       </c>
-      <c r="B109" s="38" t="s">
+      <c r="B109" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="39"/>
-      <c r="D109" s="38" t="s">
+      <c r="C109" s="36"/>
+      <c r="D109" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E109" s="39"/>
+      <c r="E109" s="36"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
         <v>8</v>
       </c>
-      <c r="B110" s="38" t="s">
+      <c r="B110" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C110" s="39"/>
-      <c r="D110" s="38" t="s">
+      <c r="C110" s="36"/>
+      <c r="D110" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="39"/>
+      <c r="E110" s="36"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="22">
         <v>10</v>
       </c>
-      <c r="B111" s="38" t="s">
+      <c r="B111" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="39"/>
-      <c r="D111" s="38" t="s">
+      <c r="C111" s="36"/>
+      <c r="D111" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="39"/>
+      <c r="E111" s="36"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="22">
         <v>11</v>
       </c>
-      <c r="B112" s="38" t="s">
+      <c r="B112" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C112" s="39"/>
-      <c r="D112" s="38" t="s">
+      <c r="C112" s="36"/>
+      <c r="D112" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E112" s="39"/>
+      <c r="E112" s="36"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="22">
         <v>12</v>
       </c>
-      <c r="B113" s="38" t="s">
+      <c r="B113" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="39"/>
-      <c r="D113" s="38" t="s">
+      <c r="C113" s="36"/>
+      <c r="D113" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E113" s="39"/>
+      <c r="E113" s="36"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="22">
         <v>13</v>
       </c>
-      <c r="B114" s="38" t="s">
+      <c r="B114" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C114" s="39"/>
-      <c r="D114" s="38" t="s">
+      <c r="C114" s="36"/>
+      <c r="D114" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="39"/>
+      <c r="E114" s="36"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="22">
         <v>14</v>
       </c>
-      <c r="B115" s="38" t="s">
+      <c r="B115" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C115" s="39"/>
-      <c r="D115" s="38" t="s">
+      <c r="C115" s="36"/>
+      <c r="D115" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E115" s="39"/>
+      <c r="E115" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="164">
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="L103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:M104"/>
+    <mergeCell ref="N104:O104"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="L100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B99:E100"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:C28"/>
@@ -3342,146 +3497,6 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B99:E100"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="H48:O48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="N99:O99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="L100:M100"/>
-    <mergeCell ref="N100:O100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="L103:M103"/>
-    <mergeCell ref="N103:O103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:M104"/>
-    <mergeCell ref="N104:O104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Añadido Documento Caso de Prueba ejecutado
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F719B-EEBE-8F40-8BA5-6C062C365A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35677677-FC50-4B47-9A57-3F4C63CA2858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC" sheetId="1" r:id="rId1"/>
+    <sheet name="Resultado Ejecucion" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="111">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -303,13 +304,79 @@
   </si>
   <si>
     <t>Deja registrar sin campo ciudad</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description / Overview</t>
+  </si>
+  <si>
+    <t>Reproduction Steps</t>
+  </si>
+  <si>
+    <t>Expected Behavior</t>
+  </si>
+  <si>
+    <t>Actual Behavior</t>
+  </si>
+  <si>
+    <t>Incidence / Severity / Probability of reproduction</t>
+  </si>
+  <si>
+    <t>100% reproduction rate</t>
+  </si>
+  <si>
+    <t>Story and Acceptance Criteria affected</t>
+  </si>
+  <si>
+    <t>Browsers tested</t>
+  </si>
+  <si>
+    <t>Google Chrome, v107</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA environment, https://demo.opencart.com/ </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Registering account is not fullfilling all requierements</t>
+  </si>
+  <si>
+    <t>Birth Date should be required but isn´t, and you can use an existing email</t>
+  </si>
+  <si>
+    <t>2- Register Account following the steps of TC-1601</t>
+  </si>
+  <si>
+    <t>3- Click register</t>
+  </si>
+  <si>
+    <t>1- Open the application page https://demo.opencart.com/register</t>
+  </si>
+  <si>
+    <t>The user is alerted that he must add a Birth Date and can´t use existing email</t>
+  </si>
+  <si>
+    <t>The user is registered</t>
+  </si>
+  <si>
+    <t>Critical severity - Missing Customer Data and Multiple registered customers with same email</t>
+  </si>
+  <si>
+    <t>Affected User Story: US-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -404,6 +471,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -440,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -713,6 +788,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -721,7 +829,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -821,62 +929,81 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1198,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101:I101"/>
+    <sheetView zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1219,10 +1346,10 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1291,16 +1418,16 @@
       <c r="E8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1315,22 +1442,22 @@
       <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51" t="s">
+      <c r="H9" s="37"/>
+      <c r="I9" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51" t="s">
+      <c r="J9" s="37"/>
+      <c r="K9" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51" t="s">
+      <c r="L9" s="37"/>
+      <c r="M9" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="51"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1345,22 +1472,22 @@
       <c r="E10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="52" t="s">
+      <c r="H10" s="39"/>
+      <c r="I10" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="52" t="s">
+      <c r="J10" s="39"/>
+      <c r="K10" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="M10" s="52" t="s">
+      <c r="L10" s="39"/>
+      <c r="M10" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="N10" s="53"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
@@ -1678,12 +1805,12 @@
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="46"/>
       <c r="G21" s="31" t="s">
         <v>74</v>
       </c>
@@ -1711,10 +1838,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="44"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="49"/>
       <c r="G22" s="31" t="s">
         <v>74</v>
       </c>
@@ -1744,10 +1871,10 @@
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="46"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="19" t="s">
         <v>14</v>
       </c>
@@ -1846,230 +1973,230 @@
       <c r="A26" s="22">
         <v>1</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35" t="s">
+      <c r="C26" s="41"/>
+      <c r="D26" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="36"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>2</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="35" t="s">
+      <c r="C27" s="41"/>
+      <c r="D27" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>4</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="35" t="s">
+      <c r="C28" s="41"/>
+      <c r="D28" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="G28" s="49" t="s">
+      <c r="E28" s="41"/>
+      <c r="G28" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49" t="s">
+      <c r="H28" s="36"/>
+      <c r="I28" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49" t="s">
+      <c r="J28" s="36"/>
+      <c r="K28" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49" t="s">
+      <c r="L28" s="36"/>
+      <c r="M28" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="N28" s="49"/>
+      <c r="N28" s="36"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>5</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="41"/>
+      <c r="D29" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="G29" s="50" t="s">
+      <c r="E29" s="41"/>
+      <c r="G29" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="50"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
     </row>
     <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>6</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="G30" s="50" t="s">
+      <c r="E30" s="41"/>
+      <c r="G30" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>7</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="35" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
+      <c r="E31" s="41"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>8</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="41"/>
+      <c r="D32" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
+      <c r="E32" s="41"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>9</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="41"/>
+      <c r="D33" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
+      <c r="E33" s="41"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
     </row>
     <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>10</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="36"/>
+      <c r="E34" s="41"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>11</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="35" t="s">
+      <c r="C35" s="41"/>
+      <c r="D35" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="36"/>
+      <c r="E35" s="41"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>12</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="35" t="s">
+      <c r="C36" s="41"/>
+      <c r="D36" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="36"/>
+      <c r="E36" s="41"/>
     </row>
     <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>13</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="35" t="s">
+      <c r="C37" s="41"/>
+      <c r="D37" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="36"/>
+      <c r="E37" s="41"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>14</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="35" t="s">
+      <c r="C38" s="41"/>
+      <c r="D38" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="41"/>
     </row>
     <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2090,20 +2217,20 @@
       <c r="C48" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="H48" s="51" t="s">
+      <c r="E48" s="53"/>
+      <c r="H48" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="51"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
     </row>
     <row r="49" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -2118,22 +2245,22 @@
       <c r="D49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="51" t="s">
+      <c r="H49" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51" t="s">
+      <c r="I49" s="37"/>
+      <c r="J49" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51" t="s">
+      <c r="K49" s="37"/>
+      <c r="L49" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51" t="s">
+      <c r="M49" s="37"/>
+      <c r="N49" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="O49" s="51"/>
+      <c r="O49" s="37"/>
     </row>
     <row r="50" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -2147,22 +2274,22 @@
       <c r="E50" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="52" t="s">
+      <c r="H50" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="53"/>
-      <c r="J50" s="52" t="s">
+      <c r="I50" s="39"/>
+      <c r="J50" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="K50" s="53"/>
-      <c r="L50" s="52" t="s">
+      <c r="K50" s="39"/>
+      <c r="L50" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="M50" s="53"/>
-      <c r="N50" s="52" t="s">
+      <c r="M50" s="39"/>
+      <c r="N50" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="O50" s="53"/>
+      <c r="O50" s="39"/>
     </row>
     <row r="51" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H51" s="30" t="s">
@@ -2324,22 +2451,22 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="17"/>
-      <c r="H57" s="49" t="s">
+      <c r="H57" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="I57" s="49"/>
-      <c r="J57" s="49" t="s">
+      <c r="I57" s="36"/>
+      <c r="J57" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="K57" s="49"/>
-      <c r="L57" s="49" t="s">
+      <c r="K57" s="36"/>
+      <c r="L57" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="M57" s="49"/>
-      <c r="N57" s="49" t="s">
+      <c r="M57" s="36"/>
+      <c r="N57" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="49"/>
+      <c r="O57" s="36"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
@@ -2348,79 +2475,79 @@
       <c r="B58" s="17"/>
       <c r="D58" s="18"/>
       <c r="E58" s="17"/>
-      <c r="H58" s="50" t="s">
+      <c r="H58" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="50"/>
-      <c r="L58" s="50"/>
-      <c r="M58" s="50"/>
-      <c r="N58" s="50"/>
-      <c r="O58" s="50"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35"/>
+      <c r="N58" s="35"/>
+      <c r="O58" s="35"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="50"/>
-      <c r="L59" s="50"/>
-      <c r="M59" s="50"/>
-      <c r="N59" s="50"/>
-      <c r="O59" s="50"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H60" s="50"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="50"/>
-      <c r="L60" s="50"/>
-      <c r="M60" s="50"/>
-      <c r="N60" s="50"/>
-      <c r="O60" s="50"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
+      <c r="O60" s="35"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="41"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="50"/>
-      <c r="M61" s="50"/>
-      <c r="N61" s="50"/>
-      <c r="O61" s="50"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="46"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="35"/>
+      <c r="N61" s="35"/>
+      <c r="O61" s="35"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="24"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="44"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="50"/>
-      <c r="J62" s="50"/>
-      <c r="K62" s="50"/>
-      <c r="L62" s="50"/>
-      <c r="M62" s="50"/>
-      <c r="N62" s="50"/>
-      <c r="O62" s="50"/>
+      <c r="B62" s="47"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="49"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
     </row>
     <row r="63" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="46"/>
+      <c r="C63" s="43"/>
       <c r="D63" s="19" t="s">
         <v>14</v>
       </c>
@@ -2445,40 +2572,40 @@
       <c r="A66" s="22">
         <v>1</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="35" t="s">
+      <c r="C66" s="41"/>
+      <c r="D66" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="36"/>
+      <c r="E66" s="41"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>2</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="35" t="s">
+      <c r="C67" s="41"/>
+      <c r="D67" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E67" s="36"/>
+      <c r="E67" s="41"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="22">
         <v>3</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="35" t="s">
+      <c r="C68" s="41"/>
+      <c r="D68" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="36"/>
+      <c r="E68" s="41"/>
     </row>
     <row r="71" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -2490,16 +2617,16 @@
     </row>
     <row r="78" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H79" s="51" t="s">
+      <c r="H79" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="I79" s="51"/>
-      <c r="J79" s="51"/>
-      <c r="K79" s="51"/>
-      <c r="L79" s="51"/>
-      <c r="M79" s="51"/>
-      <c r="N79" s="51"/>
-      <c r="O79" s="51"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="37"/>
+      <c r="O79" s="37"/>
     </row>
     <row r="80" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2511,26 +2638,26 @@
       <c r="C80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="47" t="s">
+      <c r="D80" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E80" s="48"/>
-      <c r="H80" s="51" t="s">
+      <c r="E80" s="51"/>
+      <c r="H80" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="I80" s="51"/>
-      <c r="J80" s="51" t="s">
+      <c r="I80" s="37"/>
+      <c r="J80" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="K80" s="51"/>
-      <c r="L80" s="51" t="s">
+      <c r="K80" s="37"/>
+      <c r="L80" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="M80" s="51"/>
-      <c r="N80" s="51" t="s">
+      <c r="M80" s="37"/>
+      <c r="N80" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="O80" s="51"/>
+      <c r="O80" s="37"/>
     </row>
     <row r="81" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2545,22 +2672,22 @@
       <c r="D81" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H81" s="52" t="s">
+      <c r="H81" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="I81" s="53"/>
-      <c r="J81" s="52" t="s">
+      <c r="I81" s="39"/>
+      <c r="J81" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="K81" s="53"/>
-      <c r="L81" s="52" t="s">
+      <c r="K81" s="39"/>
+      <c r="L81" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="M81" s="53"/>
-      <c r="N81" s="52" t="s">
+      <c r="M81" s="39"/>
+      <c r="N81" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="O81" s="53"/>
+      <c r="O81" s="39"/>
     </row>
     <row r="82" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -3073,78 +3200,78 @@
       <c r="A99" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="39" t="s">
+      <c r="B99" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="40"/>
-      <c r="D99" s="40"/>
-      <c r="E99" s="41"/>
-      <c r="H99" s="49" t="s">
+      <c r="C99" s="45"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="46"/>
+      <c r="H99" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="I99" s="49"/>
-      <c r="J99" s="49" t="s">
+      <c r="I99" s="36"/>
+      <c r="J99" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="K99" s="49"/>
-      <c r="L99" s="49" t="s">
+      <c r="K99" s="36"/>
+      <c r="L99" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="M99" s="49"/>
-      <c r="N99" s="49" t="s">
+      <c r="M99" s="36"/>
+      <c r="N99" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="O99" s="49"/>
+      <c r="O99" s="36"/>
     </row>
     <row r="100" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24"/>
-      <c r="B100" s="42"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-      <c r="E100" s="44"/>
-      <c r="H100" s="50" t="s">
+      <c r="B100" s="47"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="48"/>
+      <c r="E100" s="49"/>
+      <c r="H100" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I100" s="50"/>
-      <c r="J100" s="50"/>
-      <c r="K100" s="50"/>
-      <c r="L100" s="50"/>
-      <c r="M100" s="50"/>
-      <c r="N100" s="50"/>
-      <c r="O100" s="50"/>
+      <c r="I100" s="35"/>
+      <c r="J100" s="35"/>
+      <c r="K100" s="35"/>
+      <c r="L100" s="35"/>
+      <c r="M100" s="35"/>
+      <c r="N100" s="35"/>
+      <c r="O100" s="35"/>
     </row>
     <row r="101" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B101" s="45" t="s">
+      <c r="B101" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="46"/>
+      <c r="C101" s="43"/>
       <c r="D101" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H101" s="50"/>
-      <c r="I101" s="50"/>
-      <c r="J101" s="50"/>
-      <c r="K101" s="50"/>
-      <c r="L101" s="50"/>
-      <c r="M101" s="50"/>
-      <c r="N101" s="50"/>
-      <c r="O101" s="50"/>
+      <c r="H101" s="35"/>
+      <c r="I101" s="35"/>
+      <c r="J101" s="35"/>
+      <c r="K101" s="35"/>
+      <c r="L101" s="35"/>
+      <c r="M101" s="35"/>
+      <c r="N101" s="35"/>
+      <c r="O101" s="35"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H102" s="50"/>
-      <c r="I102" s="50"/>
-      <c r="J102" s="50"/>
-      <c r="K102" s="50"/>
-      <c r="L102" s="50"/>
-      <c r="M102" s="50"/>
-      <c r="N102" s="50"/>
-      <c r="O102" s="50"/>
+      <c r="H102" s="35"/>
+      <c r="I102" s="35"/>
+      <c r="J102" s="35"/>
+      <c r="K102" s="35"/>
+      <c r="L102" s="35"/>
+      <c r="M102" s="35"/>
+      <c r="N102" s="35"/>
+      <c r="O102" s="35"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
@@ -3158,321 +3285,181 @@
         <v>18</v>
       </c>
       <c r="E103" s="28"/>
-      <c r="H103" s="50"/>
-      <c r="I103" s="50"/>
-      <c r="J103" s="50"/>
-      <c r="K103" s="50"/>
-      <c r="L103" s="50"/>
-      <c r="M103" s="50"/>
-      <c r="N103" s="50"/>
-      <c r="O103" s="50"/>
+      <c r="H103" s="35"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="22">
         <v>1</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="36"/>
-      <c r="D104" s="35" t="s">
+      <c r="C104" s="41"/>
+      <c r="D104" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E104" s="36"/>
-      <c r="H104" s="50"/>
-      <c r="I104" s="50"/>
-      <c r="J104" s="50"/>
-      <c r="K104" s="50"/>
-      <c r="L104" s="50"/>
-      <c r="M104" s="50"/>
-      <c r="N104" s="50"/>
-      <c r="O104" s="50"/>
+      <c r="E104" s="41"/>
+      <c r="H104" s="35"/>
+      <c r="I104" s="35"/>
+      <c r="J104" s="35"/>
+      <c r="K104" s="35"/>
+      <c r="L104" s="35"/>
+      <c r="M104" s="35"/>
+      <c r="N104" s="35"/>
+      <c r="O104" s="35"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>2</v>
       </c>
-      <c r="B105" s="35" t="s">
+      <c r="B105" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="36"/>
-      <c r="D105" s="35" t="s">
+      <c r="C105" s="41"/>
+      <c r="D105" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="36"/>
+      <c r="E105" s="41"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
         <v>4</v>
       </c>
-      <c r="B106" s="35" t="s">
+      <c r="B106" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="36"/>
-      <c r="D106" s="35" t="s">
+      <c r="C106" s="41"/>
+      <c r="D106" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="36"/>
+      <c r="E106" s="41"/>
     </row>
     <row r="107" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22">
         <v>5</v>
       </c>
-      <c r="B107" s="35" t="s">
+      <c r="B107" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="36"/>
-      <c r="D107" s="35" t="s">
+      <c r="C107" s="41"/>
+      <c r="D107" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E107" s="36"/>
+      <c r="E107" s="41"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="22">
         <v>6</v>
       </c>
-      <c r="B108" s="35" t="s">
+      <c r="B108" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C108" s="36"/>
-      <c r="D108" s="35" t="s">
+      <c r="C108" s="41"/>
+      <c r="D108" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E108" s="36"/>
+      <c r="E108" s="41"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="22">
         <v>7</v>
       </c>
-      <c r="B109" s="35" t="s">
+      <c r="B109" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="36"/>
-      <c r="D109" s="35" t="s">
+      <c r="C109" s="41"/>
+      <c r="D109" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E109" s="36"/>
+      <c r="E109" s="41"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
         <v>8</v>
       </c>
-      <c r="B110" s="35" t="s">
+      <c r="B110" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C110" s="36"/>
-      <c r="D110" s="35" t="s">
+      <c r="C110" s="41"/>
+      <c r="D110" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="36"/>
+      <c r="E110" s="41"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="22">
         <v>10</v>
       </c>
-      <c r="B111" s="35" t="s">
+      <c r="B111" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="36"/>
-      <c r="D111" s="35" t="s">
+      <c r="C111" s="41"/>
+      <c r="D111" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="36"/>
+      <c r="E111" s="41"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="22">
         <v>11</v>
       </c>
-      <c r="B112" s="35" t="s">
+      <c r="B112" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C112" s="36"/>
-      <c r="D112" s="35" t="s">
+      <c r="C112" s="41"/>
+      <c r="D112" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E112" s="36"/>
+      <c r="E112" s="41"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="22">
         <v>12</v>
       </c>
-      <c r="B113" s="35" t="s">
+      <c r="B113" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="36"/>
-      <c r="D113" s="35" t="s">
+      <c r="C113" s="41"/>
+      <c r="D113" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E113" s="36"/>
+      <c r="E113" s="41"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="22">
         <v>13</v>
       </c>
-      <c r="B114" s="35" t="s">
+      <c r="B114" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C114" s="36"/>
-      <c r="D114" s="35" t="s">
+      <c r="C114" s="41"/>
+      <c r="D114" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="36"/>
+      <c r="E114" s="41"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="22">
         <v>14</v>
       </c>
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C115" s="36"/>
-      <c r="D115" s="35" t="s">
+      <c r="C115" s="41"/>
+      <c r="D115" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E115" s="36"/>
+      <c r="E115" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="164">
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="L103:M103"/>
-    <mergeCell ref="N103:O103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:M104"/>
-    <mergeCell ref="N104:O104"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="N99:O99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="L100:M100"/>
-    <mergeCell ref="N100:O100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="H48:O48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B99:E100"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:C28"/>
@@ -3497,7 +3484,262 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B99:E100"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="L100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="L103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:M104"/>
+    <mergeCell ref="N104:O104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C798746-2980-3444-AD9A-918694AA6428}">
+  <dimension ref="B2:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="57"/>
+      <c r="C7" s="58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="59"/>
+      <c r="C8" s="60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="59"/>
+      <c r="C15" s="60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="64"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Documentado Ejecucion de Test Case 1 y 2
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35677677-FC50-4B47-9A57-3F4C63CA2858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4157C66B-6F94-2342-8340-434B3630516F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
   <sheets>
     <sheet name="TC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="117">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -300,9 +300,6 @@
     <t>No pide Fecha Nac</t>
   </si>
   <si>
-    <t>Pide registrar con correo existente</t>
-  </si>
-  <si>
     <t>Deja registrar sin campo ciudad</t>
   </si>
   <si>
@@ -345,31 +342,52 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Registering account is not fullfilling all requierements</t>
-  </si>
-  <si>
-    <t>Birth Date should be required but isn´t, and you can use an existing email</t>
-  </si>
-  <si>
-    <t>2- Register Account following the steps of TC-1601</t>
-  </si>
-  <si>
-    <t>3- Click register</t>
-  </si>
-  <si>
-    <t>1- Open the application page https://demo.opencart.com/register</t>
-  </si>
-  <si>
-    <t>The user is alerted that he must add a Birth Date and can´t use existing email</t>
-  </si>
-  <si>
-    <t>The user is registered</t>
-  </si>
-  <si>
-    <t>Critical severity - Missing Customer Data and Multiple registered customers with same email</t>
-  </si>
-  <si>
     <t>Affected User Story: US-16</t>
+  </si>
+  <si>
+    <t>Birth Date field not asked for when registering</t>
+  </si>
+  <si>
+    <t>Birth Date should be a required field to fill when doing the registering form but it doesn´t appear</t>
+  </si>
+  <si>
+    <t>The user can fill the Birth Date field</t>
+  </si>
+  <si>
+    <t>The Birth Date field doesn´t exist</t>
+  </si>
+  <si>
+    <t>User can register new account with existing email</t>
+  </si>
+  <si>
+    <t>When registering a new account an unexisting email should be userd, otherwise it shows an error</t>
+  </si>
+  <si>
+    <t>The user is informed that the email is already in use and can´t register</t>
+  </si>
+  <si>
+    <t>The user can register with an existing email</t>
+  </si>
+  <si>
+    <t>Critical severity - Multiple accounts have the same email account</t>
+  </si>
+  <si>
+    <t>You can log in to the new account if you use its password, and to the previously existing account if you use that account´s password</t>
+  </si>
+  <si>
+    <t>Not all required fields have to be filled</t>
+  </si>
+  <si>
+    <t>The City field is a required field to fill but the system doesn´t make the user do it</t>
+  </si>
+  <si>
+    <t>The page informs the user to fill the City Field</t>
+  </si>
+  <si>
+    <t>The user is registered anyways</t>
+  </si>
+  <si>
+    <t>Critical severity - Missing Essential Customer Data</t>
   </si>
 </sst>
 </file>
@@ -515,7 +533,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -798,15 +816,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -829,7 +838,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -929,73 +938,15 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1004,6 +955,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1325,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E22"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1346,10 +1354,10 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="53"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1418,16 +1426,16 @@
       <c r="E8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
     </row>
     <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1442,22 +1450,22 @@
       <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37" t="s">
+      <c r="H9" s="61"/>
+      <c r="I9" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37" t="s">
+      <c r="J9" s="61"/>
+      <c r="K9" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37" t="s">
+      <c r="L9" s="61"/>
+      <c r="M9" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="37"/>
+      <c r="N9" s="61"/>
     </row>
     <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1472,22 +1480,22 @@
       <c r="E10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="38" t="s">
+      <c r="H10" s="63"/>
+      <c r="I10" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="38" t="s">
+      <c r="J10" s="63"/>
+      <c r="K10" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="38" t="s">
+      <c r="L10" s="63"/>
+      <c r="M10" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="N10" s="39"/>
+      <c r="N10" s="63"/>
     </row>
     <row r="11" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
@@ -1805,12 +1813,12 @@
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
       <c r="G21" s="31" t="s">
         <v>74</v>
       </c>
@@ -1838,10 +1846,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="54"/>
       <c r="G22" s="31" t="s">
         <v>74</v>
       </c>
@@ -1871,10 +1879,10 @@
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="43"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="19" t="s">
         <v>14</v>
       </c>
@@ -1973,230 +1981,228 @@
       <c r="A26" s="22">
         <v>1</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="40" t="s">
+      <c r="C26" s="46"/>
+      <c r="D26" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="41"/>
+      <c r="E26" s="46"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>2</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="40" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="46"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>4</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="40" t="s">
+      <c r="C28" s="46"/>
+      <c r="D28" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="G28" s="36" t="s">
+      <c r="E28" s="46"/>
+      <c r="G28" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36" t="s">
+      <c r="H28" s="59"/>
+      <c r="I28" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36" t="s">
+      <c r="J28" s="59"/>
+      <c r="K28" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36" t="s">
+      <c r="L28" s="59"/>
+      <c r="M28" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="N28" s="36"/>
+      <c r="N28" s="59"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>5</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="40" t="s">
+      <c r="C29" s="46"/>
+      <c r="D29" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="G29" s="35" t="s">
+      <c r="E29" s="46"/>
+      <c r="G29" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
     </row>
     <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>6</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="40" t="s">
+      <c r="C30" s="46"/>
+      <c r="D30" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="41"/>
-      <c r="G30" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
+      <c r="E30" s="46"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>7</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="40" t="s">
+      <c r="C31" s="46"/>
+      <c r="D31" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
+      <c r="E31" s="46"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>8</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="40" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
+      <c r="E32" s="46"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>9</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="40" t="s">
+      <c r="C33" s="46"/>
+      <c r="D33" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="41"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
+      <c r="E33" s="46"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
     </row>
     <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>10</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="40" t="s">
+      <c r="C34" s="46"/>
+      <c r="D34" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="41"/>
+      <c r="E34" s="46"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>11</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="40" t="s">
+      <c r="C35" s="46"/>
+      <c r="D35" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="41"/>
+      <c r="E35" s="46"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>12</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="40" t="s">
+      <c r="C36" s="46"/>
+      <c r="D36" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="41"/>
+      <c r="E36" s="46"/>
     </row>
     <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>13</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="40" t="s">
+      <c r="C37" s="46"/>
+      <c r="D37" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="41"/>
+      <c r="E37" s="46"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>14</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="40" t="s">
+      <c r="C38" s="46"/>
+      <c r="D38" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="41"/>
+      <c r="E38" s="46"/>
     </row>
     <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2217,20 +2223,20 @@
       <c r="C48" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="52" t="s">
+      <c r="D48" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="53"/>
-      <c r="H48" s="37" t="s">
+      <c r="E48" s="48"/>
+      <c r="H48" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="61"/>
     </row>
     <row r="49" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -2245,22 +2251,22 @@
       <c r="D49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="H49" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37" t="s">
+      <c r="I49" s="61"/>
+      <c r="J49" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37" t="s">
+      <c r="K49" s="61"/>
+      <c r="L49" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37" t="s">
+      <c r="M49" s="61"/>
+      <c r="N49" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="O49" s="37"/>
+      <c r="O49" s="61"/>
     </row>
     <row r="50" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -2274,22 +2280,22 @@
       <c r="E50" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="38" t="s">
+      <c r="H50" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="39"/>
-      <c r="J50" s="38" t="s">
+      <c r="I50" s="63"/>
+      <c r="J50" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="K50" s="39"/>
-      <c r="L50" s="38" t="s">
+      <c r="K50" s="63"/>
+      <c r="L50" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="M50" s="39"/>
-      <c r="N50" s="38" t="s">
+      <c r="M50" s="63"/>
+      <c r="N50" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="O50" s="39"/>
+      <c r="O50" s="63"/>
     </row>
     <row r="51" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H51" s="30" t="s">
@@ -2451,22 +2457,22 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="17"/>
-      <c r="H57" s="36" t="s">
+      <c r="H57" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36" t="s">
+      <c r="I57" s="59"/>
+      <c r="J57" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="K57" s="36"/>
-      <c r="L57" s="36" t="s">
+      <c r="K57" s="59"/>
+      <c r="L57" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M57" s="36"/>
-      <c r="N57" s="36" t="s">
+      <c r="M57" s="59"/>
+      <c r="N57" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="36"/>
+      <c r="O57" s="59"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
@@ -2475,79 +2481,79 @@
       <c r="B58" s="17"/>
       <c r="D58" s="18"/>
       <c r="E58" s="17"/>
-      <c r="H58" s="35" t="s">
+      <c r="H58" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35"/>
-      <c r="O58" s="35"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="60"/>
+      <c r="K58" s="60"/>
+      <c r="L58" s="60"/>
+      <c r="M58" s="60"/>
+      <c r="N58" s="60"/>
+      <c r="O58" s="60"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="35"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="60"/>
+      <c r="N59" s="60"/>
+      <c r="O59" s="60"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="60"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="60"/>
+      <c r="N60" s="60"/>
+      <c r="O60" s="60"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="46"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
-      <c r="O61" s="35"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="51"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="60"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="24"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="49"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
-      <c r="O62" s="35"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="54"/>
+      <c r="H62" s="60"/>
+      <c r="I62" s="60"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="60"/>
+      <c r="M62" s="60"/>
+      <c r="N62" s="60"/>
+      <c r="O62" s="60"/>
     </row>
     <row r="63" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="43"/>
+      <c r="C63" s="56"/>
       <c r="D63" s="19" t="s">
         <v>14</v>
       </c>
@@ -2572,40 +2578,40 @@
       <c r="A66" s="22">
         <v>1</v>
       </c>
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="40" t="s">
+      <c r="C66" s="46"/>
+      <c r="D66" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="41"/>
+      <c r="E66" s="46"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>2</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="41"/>
-      <c r="D67" s="40" t="s">
+      <c r="C67" s="46"/>
+      <c r="D67" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E67" s="41"/>
+      <c r="E67" s="46"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="22">
         <v>3</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="41"/>
-      <c r="D68" s="40" t="s">
+      <c r="C68" s="46"/>
+      <c r="D68" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="41"/>
+      <c r="E68" s="46"/>
     </row>
     <row r="71" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -2617,16 +2623,16 @@
     </row>
     <row r="78" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H79" s="37" t="s">
+      <c r="H79" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="I79" s="37"/>
-      <c r="J79" s="37"/>
-      <c r="K79" s="37"/>
-      <c r="L79" s="37"/>
-      <c r="M79" s="37"/>
-      <c r="N79" s="37"/>
-      <c r="O79" s="37"/>
+      <c r="I79" s="61"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
+      <c r="L79" s="61"/>
+      <c r="M79" s="61"/>
+      <c r="N79" s="61"/>
+      <c r="O79" s="61"/>
     </row>
     <row r="80" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2638,26 +2644,26 @@
       <c r="C80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="50" t="s">
+      <c r="D80" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E80" s="51"/>
-      <c r="H80" s="37" t="s">
+      <c r="E80" s="58"/>
+      <c r="H80" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="I80" s="37"/>
-      <c r="J80" s="37" t="s">
+      <c r="I80" s="61"/>
+      <c r="J80" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="K80" s="37"/>
-      <c r="L80" s="37" t="s">
+      <c r="K80" s="61"/>
+      <c r="L80" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="M80" s="37"/>
-      <c r="N80" s="37" t="s">
+      <c r="M80" s="61"/>
+      <c r="N80" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="O80" s="37"/>
+      <c r="O80" s="61"/>
     </row>
     <row r="81" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2672,22 +2678,22 @@
       <c r="D81" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H81" s="38" t="s">
+      <c r="H81" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="I81" s="39"/>
-      <c r="J81" s="38" t="s">
+      <c r="I81" s="63"/>
+      <c r="J81" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="K81" s="39"/>
-      <c r="L81" s="38" t="s">
+      <c r="K81" s="63"/>
+      <c r="L81" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="M81" s="39"/>
-      <c r="N81" s="38" t="s">
+      <c r="M81" s="63"/>
+      <c r="N81" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="O81" s="39"/>
+      <c r="O81" s="63"/>
     </row>
     <row r="82" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -3200,78 +3206,78 @@
       <c r="A99" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="44" t="s">
+      <c r="B99" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="46"/>
-      <c r="H99" s="36" t="s">
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="51"/>
+      <c r="H99" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36" t="s">
+      <c r="I99" s="59"/>
+      <c r="J99" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="K99" s="36"/>
-      <c r="L99" s="36" t="s">
+      <c r="K99" s="59"/>
+      <c r="L99" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M99" s="36"/>
-      <c r="N99" s="36" t="s">
+      <c r="M99" s="59"/>
+      <c r="N99" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="O99" s="36"/>
+      <c r="O99" s="59"/>
     </row>
     <row r="100" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24"/>
-      <c r="B100" s="47"/>
-      <c r="C100" s="48"/>
-      <c r="D100" s="48"/>
-      <c r="E100" s="49"/>
-      <c r="H100" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="I100" s="35"/>
-      <c r="J100" s="35"/>
-      <c r="K100" s="35"/>
-      <c r="L100" s="35"/>
-      <c r="M100" s="35"/>
-      <c r="N100" s="35"/>
-      <c r="O100" s="35"/>
+      <c r="B100" s="52"/>
+      <c r="C100" s="53"/>
+      <c r="D100" s="53"/>
+      <c r="E100" s="54"/>
+      <c r="H100" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="I100" s="60"/>
+      <c r="J100" s="60"/>
+      <c r="K100" s="60"/>
+      <c r="L100" s="60"/>
+      <c r="M100" s="60"/>
+      <c r="N100" s="60"/>
+      <c r="O100" s="60"/>
     </row>
     <row r="101" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B101" s="42" t="s">
+      <c r="B101" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="43"/>
+      <c r="C101" s="56"/>
       <c r="D101" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H101" s="35"/>
-      <c r="I101" s="35"/>
-      <c r="J101" s="35"/>
-      <c r="K101" s="35"/>
-      <c r="L101" s="35"/>
-      <c r="M101" s="35"/>
-      <c r="N101" s="35"/>
-      <c r="O101" s="35"/>
+      <c r="H101" s="60"/>
+      <c r="I101" s="60"/>
+      <c r="J101" s="60"/>
+      <c r="K101" s="60"/>
+      <c r="L101" s="60"/>
+      <c r="M101" s="60"/>
+      <c r="N101" s="60"/>
+      <c r="O101" s="60"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H102" s="35"/>
-      <c r="I102" s="35"/>
-      <c r="J102" s="35"/>
-      <c r="K102" s="35"/>
-      <c r="L102" s="35"/>
-      <c r="M102" s="35"/>
-      <c r="N102" s="35"/>
-      <c r="O102" s="35"/>
+      <c r="H102" s="60"/>
+      <c r="I102" s="60"/>
+      <c r="J102" s="60"/>
+      <c r="K102" s="60"/>
+      <c r="L102" s="60"/>
+      <c r="M102" s="60"/>
+      <c r="N102" s="60"/>
+      <c r="O102" s="60"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
@@ -3285,181 +3291,321 @@
         <v>18</v>
       </c>
       <c r="E103" s="28"/>
-      <c r="H103" s="35"/>
-      <c r="I103" s="35"/>
-      <c r="J103" s="35"/>
-      <c r="K103" s="35"/>
-      <c r="L103" s="35"/>
-      <c r="M103" s="35"/>
-      <c r="N103" s="35"/>
-      <c r="O103" s="35"/>
+      <c r="H103" s="60"/>
+      <c r="I103" s="60"/>
+      <c r="J103" s="60"/>
+      <c r="K103" s="60"/>
+      <c r="L103" s="60"/>
+      <c r="M103" s="60"/>
+      <c r="N103" s="60"/>
+      <c r="O103" s="60"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="22">
         <v>1</v>
       </c>
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="41"/>
-      <c r="D104" s="40" t="s">
+      <c r="C104" s="46"/>
+      <c r="D104" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E104" s="41"/>
-      <c r="H104" s="35"/>
-      <c r="I104" s="35"/>
-      <c r="J104" s="35"/>
-      <c r="K104" s="35"/>
-      <c r="L104" s="35"/>
-      <c r="M104" s="35"/>
-      <c r="N104" s="35"/>
-      <c r="O104" s="35"/>
+      <c r="E104" s="46"/>
+      <c r="H104" s="60"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="60"/>
+      <c r="K104" s="60"/>
+      <c r="L104" s="60"/>
+      <c r="M104" s="60"/>
+      <c r="N104" s="60"/>
+      <c r="O104" s="60"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>2</v>
       </c>
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="41"/>
-      <c r="D105" s="40" t="s">
+      <c r="C105" s="46"/>
+      <c r="D105" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="41"/>
+      <c r="E105" s="46"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
         <v>4</v>
       </c>
-      <c r="B106" s="40" t="s">
+      <c r="B106" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="41"/>
-      <c r="D106" s="40" t="s">
+      <c r="C106" s="46"/>
+      <c r="D106" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="41"/>
+      <c r="E106" s="46"/>
     </row>
     <row r="107" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22">
         <v>5</v>
       </c>
-      <c r="B107" s="40" t="s">
+      <c r="B107" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="41"/>
-      <c r="D107" s="40" t="s">
+      <c r="C107" s="46"/>
+      <c r="D107" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E107" s="41"/>
+      <c r="E107" s="46"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="22">
         <v>6</v>
       </c>
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C108" s="41"/>
-      <c r="D108" s="40" t="s">
+      <c r="C108" s="46"/>
+      <c r="D108" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E108" s="41"/>
+      <c r="E108" s="46"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="22">
         <v>7</v>
       </c>
-      <c r="B109" s="40" t="s">
+      <c r="B109" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="41"/>
-      <c r="D109" s="40" t="s">
+      <c r="C109" s="46"/>
+      <c r="D109" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E109" s="41"/>
+      <c r="E109" s="46"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
         <v>8</v>
       </c>
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C110" s="41"/>
-      <c r="D110" s="40" t="s">
+      <c r="C110" s="46"/>
+      <c r="D110" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="41"/>
+      <c r="E110" s="46"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="22">
         <v>10</v>
       </c>
-      <c r="B111" s="40" t="s">
+      <c r="B111" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="41"/>
-      <c r="D111" s="40" t="s">
+      <c r="C111" s="46"/>
+      <c r="D111" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="41"/>
+      <c r="E111" s="46"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="22">
         <v>11</v>
       </c>
-      <c r="B112" s="40" t="s">
+      <c r="B112" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C112" s="41"/>
-      <c r="D112" s="40" t="s">
+      <c r="C112" s="46"/>
+      <c r="D112" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E112" s="41"/>
+      <c r="E112" s="46"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="22">
         <v>12</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="41"/>
-      <c r="D113" s="40" t="s">
+      <c r="C113" s="46"/>
+      <c r="D113" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E113" s="41"/>
+      <c r="E113" s="46"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="22">
         <v>13</v>
       </c>
-      <c r="B114" s="40" t="s">
+      <c r="B114" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C114" s="41"/>
-      <c r="D114" s="40" t="s">
+      <c r="C114" s="46"/>
+      <c r="D114" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="41"/>
+      <c r="E114" s="46"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="22">
         <v>14</v>
       </c>
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C115" s="41"/>
-      <c r="D115" s="40" t="s">
+      <c r="C115" s="46"/>
+      <c r="D115" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E115" s="41"/>
+      <c r="E115" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="164">
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="L103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:M104"/>
+    <mergeCell ref="N104:O104"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="L100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B99:E100"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:C28"/>
@@ -3484,146 +3630,6 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B99:E100"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="H48:O48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="N99:O99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="L100:M100"/>
-    <mergeCell ref="N100:O100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="L103:M103"/>
-    <mergeCell ref="N103:O103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:M104"/>
-    <mergeCell ref="N104:O104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3631,115 +3637,532 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C798746-2980-3444-AD9A-918694AA6428}">
-  <dimension ref="B2:C23"/>
+  <dimension ref="B2:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="55" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="38"/>
+      <c r="C7" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="39"/>
+      <c r="C8" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="46"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="46"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="46"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="46"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="46"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="46"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="46"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="46"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="46"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C20" s="42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="39"/>
+      <c r="C25" s="40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="44"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="57"/>
-      <c r="C7" s="58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="61" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="46"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="38"/>
+      <c r="C45" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="46"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="39"/>
+      <c r="C46" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="46"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="46"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="46"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="46"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="46"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="46"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="46"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="46"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="46"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="46"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="46"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="62" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="61" t="s">
+      <c r="C60" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="55" t="s">
+      <c r="C62" s="37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="39"/>
+      <c r="C63" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="59"/>
-      <c r="C15" s="60" t="s">
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" s="41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="61" t="s">
+      <c r="C65" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="61" t="s">
+      <c r="C67" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="62" t="s">
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B69" s="41" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="61" t="s">
+      <c r="C69" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="62" t="s">
+    </row>
+    <row r="71" spans="2:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B71" s="41" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="61" t="s">
+      <c r="C71" s="44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B77" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B79" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B81" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" s="46"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="38"/>
+      <c r="C82" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82" s="46"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="39"/>
+      <c r="C83" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" s="46"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C84" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" s="46"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C85" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="46"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C86" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="46"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C87" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="46"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C88" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D88" s="46"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C89" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" s="46"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C90" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" s="46"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C91" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" s="46"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C92" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" s="46"/>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B95" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C97" s="42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B99" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B100" s="39"/>
+      <c r="C100" s="40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B102" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="64"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B104" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C104" s="42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B106" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C106" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B108" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C108" s="44"/>
     </row>
   </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadido Assert en Automatizacion TC02
</commit_message>
<xml_diff>
--- a/test_cases/TC_01.xlsx
+++ b/test_cases/TC_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4157C66B-6F94-2342-8340-434B3630516F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4113DF5F-59B2-B744-A244-FC2E97F53F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{09965871-8701-0A4F-BAB9-89B468260767}"/>
   </bookViews>
@@ -838,7 +838,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -956,63 +956,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -1333,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76DCEE-79F3-5348-8653-09A99BC56BD0}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="105" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1354,10 +1355,10 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="48"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1426,16 +1427,16 @@
       <c r="E8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1450,22 +1451,22 @@
       <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61" t="s">
+      <c r="H9" s="47"/>
+      <c r="I9" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61" t="s">
+      <c r="J9" s="47"/>
+      <c r="K9" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61" t="s">
+      <c r="L9" s="47"/>
+      <c r="M9" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="61"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1480,22 +1481,22 @@
       <c r="E10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="62" t="s">
+      <c r="G10" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="62" t="s">
+      <c r="H10" s="49"/>
+      <c r="I10" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="63"/>
-      <c r="K10" s="62" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="63"/>
-      <c r="M10" s="62" t="s">
+      <c r="L10" s="49"/>
+      <c r="M10" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="N10" s="63"/>
+      <c r="N10" s="49"/>
     </row>
     <row r="11" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
@@ -1813,12 +1814,12 @@
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
       <c r="G21" s="31" t="s">
         <v>74</v>
       </c>
@@ -1846,10 +1847,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
       <c r="G22" s="31" t="s">
         <v>74</v>
       </c>
@@ -1879,10 +1880,10 @@
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="19" t="s">
         <v>14</v>
       </c>
@@ -1981,228 +1982,228 @@
       <c r="A26" s="22">
         <v>1</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="45" t="s">
+      <c r="C26" s="51"/>
+      <c r="D26" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="46"/>
+      <c r="E26" s="51"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>2</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="45" t="s">
+      <c r="C27" s="51"/>
+      <c r="D27" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="46"/>
+      <c r="E27" s="51"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>4</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="45" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="46"/>
-      <c r="G28" s="59" t="s">
+      <c r="E28" s="51"/>
+      <c r="G28" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59" t="s">
+      <c r="H28" s="46"/>
+      <c r="I28" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59" t="s">
+      <c r="J28" s="46"/>
+      <c r="K28" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59" t="s">
+      <c r="L28" s="46"/>
+      <c r="M28" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="N28" s="59"/>
+      <c r="N28" s="46"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>5</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="45" t="s">
+      <c r="C29" s="51"/>
+      <c r="D29" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="46"/>
-      <c r="G29" s="60" t="s">
+      <c r="E29" s="51"/>
+      <c r="G29" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>6</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="45" t="s">
+      <c r="C30" s="51"/>
+      <c r="D30" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
+      <c r="E30" s="51"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>7</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="45" t="s">
+      <c r="C31" s="51"/>
+      <c r="D31" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="46"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
+      <c r="E31" s="51"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>8</v>
       </c>
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="45" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
+      <c r="E32" s="51"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>9</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="45" t="s">
+      <c r="C33" s="51"/>
+      <c r="D33" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
+      <c r="E33" s="51"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
     </row>
     <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>10</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="45" t="s">
+      <c r="C34" s="51"/>
+      <c r="D34" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="46"/>
+      <c r="E34" s="51"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>11</v>
       </c>
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="45" t="s">
+      <c r="C35" s="51"/>
+      <c r="D35" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="46"/>
+      <c r="E35" s="51"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>12</v>
       </c>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="45" t="s">
+      <c r="C36" s="51"/>
+      <c r="D36" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="51"/>
     </row>
     <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>13</v>
       </c>
-      <c r="B37" s="45" t="s">
+      <c r="B37" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="45" t="s">
+      <c r="C37" s="51"/>
+      <c r="D37" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="46"/>
+      <c r="E37" s="51"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>14</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="45" t="s">
+      <c r="C38" s="51"/>
+      <c r="D38" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="46"/>
+      <c r="E38" s="51"/>
     </row>
     <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2223,20 +2224,20 @@
       <c r="C48" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="H48" s="61" t="s">
+      <c r="E48" s="63"/>
+      <c r="H48" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
     </row>
     <row r="49" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -2251,22 +2252,22 @@
       <c r="D49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="61" t="s">
+      <c r="H49" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61" t="s">
+      <c r="I49" s="47"/>
+      <c r="J49" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61" t="s">
+      <c r="K49" s="47"/>
+      <c r="L49" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="M49" s="61"/>
-      <c r="N49" s="61" t="s">
+      <c r="M49" s="47"/>
+      <c r="N49" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="O49" s="61"/>
+      <c r="O49" s="47"/>
     </row>
     <row r="50" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -2280,22 +2281,22 @@
       <c r="E50" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="62" t="s">
+      <c r="H50" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="63"/>
-      <c r="J50" s="62" t="s">
+      <c r="I50" s="49"/>
+      <c r="J50" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="K50" s="63"/>
-      <c r="L50" s="62" t="s">
+      <c r="K50" s="49"/>
+      <c r="L50" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="M50" s="63"/>
-      <c r="N50" s="62" t="s">
+      <c r="M50" s="49"/>
+      <c r="N50" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="O50" s="63"/>
+      <c r="O50" s="49"/>
     </row>
     <row r="51" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H51" s="30" t="s">
@@ -2457,22 +2458,22 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="17"/>
-      <c r="H57" s="59" t="s">
+      <c r="H57" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="I57" s="59"/>
-      <c r="J57" s="59" t="s">
+      <c r="I57" s="46"/>
+      <c r="J57" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K57" s="59"/>
-      <c r="L57" s="59" t="s">
+      <c r="K57" s="46"/>
+      <c r="L57" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="M57" s="59"/>
-      <c r="N57" s="59" t="s">
+      <c r="M57" s="46"/>
+      <c r="N57" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="59"/>
+      <c r="O57" s="46"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
@@ -2481,79 +2482,79 @@
       <c r="B58" s="17"/>
       <c r="D58" s="18"/>
       <c r="E58" s="17"/>
-      <c r="H58" s="60" t="s">
+      <c r="H58" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="60"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="60"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="60"/>
-      <c r="N58" s="60"/>
-      <c r="O58" s="60"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="45"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="60"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="60"/>
-      <c r="N59" s="60"/>
-      <c r="O59" s="60"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="45"/>
+      <c r="L59" s="45"/>
+      <c r="M59" s="45"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="45"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="60"/>
-      <c r="K60" s="60"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="60"/>
-      <c r="N60" s="60"/>
-      <c r="O60" s="60"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="45"/>
+      <c r="L60" s="45"/>
+      <c r="M60" s="45"/>
+      <c r="N60" s="45"/>
+      <c r="O60" s="45"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="51"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="60"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="60"/>
-      <c r="M61" s="60"/>
-      <c r="N61" s="60"/>
-      <c r="O61" s="60"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="56"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="45"/>
+      <c r="L61" s="45"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="45"/>
+      <c r="O61" s="45"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="24"/>
-      <c r="B62" s="52"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="54"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="60"/>
-      <c r="J62" s="60"/>
-      <c r="K62" s="60"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-      <c r="O62" s="60"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="59"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="45"/>
+      <c r="O62" s="45"/>
     </row>
     <row r="63" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="56"/>
+      <c r="C63" s="53"/>
       <c r="D63" s="19" t="s">
         <v>14</v>
       </c>
@@ -2578,40 +2579,40 @@
       <c r="A66" s="22">
         <v>1</v>
       </c>
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="46"/>
-      <c r="D66" s="45" t="s">
+      <c r="C66" s="51"/>
+      <c r="D66" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="46"/>
+      <c r="E66" s="51"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>2</v>
       </c>
-      <c r="B67" s="45" t="s">
+      <c r="B67" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="45" t="s">
+      <c r="C67" s="51"/>
+      <c r="D67" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E67" s="46"/>
+      <c r="E67" s="51"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="22">
         <v>3</v>
       </c>
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="46"/>
-      <c r="D68" s="45" t="s">
+      <c r="C68" s="51"/>
+      <c r="D68" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="46"/>
+      <c r="E68" s="51"/>
     </row>
     <row r="71" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -2623,16 +2624,16 @@
     </row>
     <row r="78" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H79" s="61" t="s">
+      <c r="H79" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="I79" s="61"/>
-      <c r="J79" s="61"/>
-      <c r="K79" s="61"/>
-      <c r="L79" s="61"/>
-      <c r="M79" s="61"/>
-      <c r="N79" s="61"/>
-      <c r="O79" s="61"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+      <c r="O79" s="47"/>
     </row>
     <row r="80" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2644,26 +2645,26 @@
       <c r="C80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="57" t="s">
+      <c r="D80" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="E80" s="58"/>
-      <c r="H80" s="61" t="s">
+      <c r="E80" s="61"/>
+      <c r="H80" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="I80" s="61"/>
-      <c r="J80" s="61" t="s">
+      <c r="I80" s="47"/>
+      <c r="J80" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="K80" s="61"/>
-      <c r="L80" s="61" t="s">
+      <c r="K80" s="47"/>
+      <c r="L80" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="M80" s="61"/>
-      <c r="N80" s="61" t="s">
+      <c r="M80" s="47"/>
+      <c r="N80" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="O80" s="61"/>
+      <c r="O80" s="47"/>
     </row>
     <row r="81" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2678,22 +2679,22 @@
       <c r="D81" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H81" s="62" t="s">
+      <c r="H81" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="I81" s="63"/>
-      <c r="J81" s="62" t="s">
+      <c r="I81" s="49"/>
+      <c r="J81" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="K81" s="63"/>
-      <c r="L81" s="62" t="s">
+      <c r="K81" s="49"/>
+      <c r="L81" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="M81" s="63"/>
-      <c r="N81" s="62" t="s">
+      <c r="M81" s="49"/>
+      <c r="N81" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="O81" s="63"/>
+      <c r="O81" s="49"/>
     </row>
     <row r="82" spans="1:15" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -3206,78 +3207,78 @@
       <c r="A99" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="49" t="s">
+      <c r="B99" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="51"/>
-      <c r="H99" s="59" t="s">
+      <c r="C99" s="55"/>
+      <c r="D99" s="55"/>
+      <c r="E99" s="56"/>
+      <c r="H99" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="I99" s="59"/>
-      <c r="J99" s="59" t="s">
+      <c r="I99" s="46"/>
+      <c r="J99" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K99" s="59"/>
-      <c r="L99" s="59" t="s">
+      <c r="K99" s="46"/>
+      <c r="L99" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="M99" s="59"/>
-      <c r="N99" s="59" t="s">
+      <c r="M99" s="46"/>
+      <c r="N99" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="O99" s="59"/>
+      <c r="O99" s="46"/>
     </row>
     <row r="100" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24"/>
-      <c r="B100" s="52"/>
-      <c r="C100" s="53"/>
-      <c r="D100" s="53"/>
-      <c r="E100" s="54"/>
-      <c r="H100" s="60" t="s">
+      <c r="B100" s="57"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="58"/>
+      <c r="E100" s="59"/>
+      <c r="H100" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="I100" s="60"/>
-      <c r="J100" s="60"/>
-      <c r="K100" s="60"/>
-      <c r="L100" s="60"/>
-      <c r="M100" s="60"/>
-      <c r="N100" s="60"/>
-      <c r="O100" s="60"/>
+      <c r="I100" s="45"/>
+      <c r="J100" s="45"/>
+      <c r="K100" s="45"/>
+      <c r="L100" s="45"/>
+      <c r="M100" s="45"/>
+      <c r="N100" s="45"/>
+      <c r="O100" s="45"/>
     </row>
     <row r="101" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B101" s="55" t="s">
+      <c r="B101" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="56"/>
+      <c r="C101" s="53"/>
       <c r="D101" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H101" s="60"/>
-      <c r="I101" s="60"/>
-      <c r="J101" s="60"/>
-      <c r="K101" s="60"/>
-      <c r="L101" s="60"/>
-      <c r="M101" s="60"/>
-      <c r="N101" s="60"/>
-      <c r="O101" s="60"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="45"/>
+      <c r="J101" s="45"/>
+      <c r="K101" s="45"/>
+      <c r="L101" s="45"/>
+      <c r="M101" s="45"/>
+      <c r="N101" s="45"/>
+      <c r="O101" s="45"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H102" s="60"/>
-      <c r="I102" s="60"/>
-      <c r="J102" s="60"/>
-      <c r="K102" s="60"/>
-      <c r="L102" s="60"/>
-      <c r="M102" s="60"/>
-      <c r="N102" s="60"/>
-      <c r="O102" s="60"/>
+      <c r="H102" s="45"/>
+      <c r="I102" s="45"/>
+      <c r="J102" s="45"/>
+      <c r="K102" s="45"/>
+      <c r="L102" s="45"/>
+      <c r="M102" s="45"/>
+      <c r="N102" s="45"/>
+      <c r="O102" s="45"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
@@ -3291,321 +3292,181 @@
         <v>18</v>
       </c>
       <c r="E103" s="28"/>
-      <c r="H103" s="60"/>
-      <c r="I103" s="60"/>
-      <c r="J103" s="60"/>
-      <c r="K103" s="60"/>
-      <c r="L103" s="60"/>
-      <c r="M103" s="60"/>
-      <c r="N103" s="60"/>
-      <c r="O103" s="60"/>
+      <c r="H103" s="45"/>
+      <c r="I103" s="45"/>
+      <c r="J103" s="45"/>
+      <c r="K103" s="45"/>
+      <c r="L103" s="45"/>
+      <c r="M103" s="45"/>
+      <c r="N103" s="45"/>
+      <c r="O103" s="45"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="22">
         <v>1</v>
       </c>
-      <c r="B104" s="45" t="s">
+      <c r="B104" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="46"/>
-      <c r="D104" s="45" t="s">
+      <c r="C104" s="51"/>
+      <c r="D104" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E104" s="46"/>
-      <c r="H104" s="60"/>
-      <c r="I104" s="60"/>
-      <c r="J104" s="60"/>
-      <c r="K104" s="60"/>
-      <c r="L104" s="60"/>
-      <c r="M104" s="60"/>
-      <c r="N104" s="60"/>
-      <c r="O104" s="60"/>
+      <c r="E104" s="51"/>
+      <c r="H104" s="45"/>
+      <c r="I104" s="45"/>
+      <c r="J104" s="45"/>
+      <c r="K104" s="45"/>
+      <c r="L104" s="45"/>
+      <c r="M104" s="45"/>
+      <c r="N104" s="45"/>
+      <c r="O104" s="45"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>2</v>
       </c>
-      <c r="B105" s="45" t="s">
+      <c r="B105" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="46"/>
-      <c r="D105" s="45" t="s">
+      <c r="C105" s="51"/>
+      <c r="D105" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="46"/>
+      <c r="E105" s="51"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
         <v>4</v>
       </c>
-      <c r="B106" s="45" t="s">
+      <c r="B106" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="46"/>
-      <c r="D106" s="45" t="s">
+      <c r="C106" s="51"/>
+      <c r="D106" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="46"/>
+      <c r="E106" s="51"/>
     </row>
     <row r="107" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22">
         <v>5</v>
       </c>
-      <c r="B107" s="45" t="s">
+      <c r="B107" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="46"/>
-      <c r="D107" s="45" t="s">
+      <c r="C107" s="51"/>
+      <c r="D107" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E107" s="46"/>
+      <c r="E107" s="51"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="22">
         <v>6</v>
       </c>
-      <c r="B108" s="45" t="s">
+      <c r="B108" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C108" s="46"/>
-      <c r="D108" s="45" t="s">
+      <c r="C108" s="51"/>
+      <c r="D108" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E108" s="46"/>
+      <c r="E108" s="51"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="22">
         <v>7</v>
       </c>
-      <c r="B109" s="45" t="s">
+      <c r="B109" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="46"/>
-      <c r="D109" s="45" t="s">
+      <c r="C109" s="51"/>
+      <c r="D109" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E109" s="46"/>
+      <c r="E109" s="51"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
         <v>8</v>
       </c>
-      <c r="B110" s="45" t="s">
+      <c r="B110" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C110" s="46"/>
-      <c r="D110" s="45" t="s">
+      <c r="C110" s="51"/>
+      <c r="D110" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="46"/>
+      <c r="E110" s="51"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="22">
         <v>10</v>
       </c>
-      <c r="B111" s="45" t="s">
+      <c r="B111" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="46"/>
-      <c r="D111" s="45" t="s">
+      <c r="C111" s="51"/>
+      <c r="D111" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="46"/>
+      <c r="E111" s="51"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="22">
         <v>11</v>
       </c>
-      <c r="B112" s="45" t="s">
+      <c r="B112" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C112" s="46"/>
-      <c r="D112" s="45" t="s">
+      <c r="C112" s="51"/>
+      <c r="D112" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E112" s="46"/>
+      <c r="E112" s="51"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="22">
         <v>12</v>
       </c>
-      <c r="B113" s="45" t="s">
+      <c r="B113" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="46"/>
-      <c r="D113" s="45" t="s">
+      <c r="C113" s="51"/>
+      <c r="D113" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E113" s="46"/>
+      <c r="E113" s="51"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="22">
         <v>13</v>
       </c>
-      <c r="B114" s="45" t="s">
+      <c r="B114" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C114" s="46"/>
-      <c r="D114" s="45" t="s">
+      <c r="C114" s="51"/>
+      <c r="D114" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="46"/>
+      <c r="E114" s="51"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="22">
         <v>14</v>
       </c>
-      <c r="B115" s="45" t="s">
+      <c r="B115" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C115" s="46"/>
-      <c r="D115" s="45" t="s">
+      <c r="C115" s="51"/>
+      <c r="D115" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E115" s="46"/>
+      <c r="E115" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="164">
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="L103:M103"/>
-    <mergeCell ref="N103:O103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:M104"/>
-    <mergeCell ref="N104:O104"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="N99:O99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="L100:M100"/>
-    <mergeCell ref="N100:O100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="H48:O48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B99:E100"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:C28"/>
@@ -3630,6 +3491,146 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B99:E100"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="L100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="L103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:M104"/>
+    <mergeCell ref="N104:O104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3637,10 +3638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C798746-2980-3444-AD9A-918694AA6428}">
-  <dimension ref="B2:D108"/>
+  <dimension ref="A2:D108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3669,84 +3670,84 @@
       <c r="B6" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="38"/>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="39"/>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="51"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="51"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="51"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="51"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="51"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="46"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="46"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="51"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="41" t="s">
@@ -3802,13 +3803,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="41" t="s">
         <v>100</v>
       </c>
       <c r="C33" s="44"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>88</v>
       </c>
@@ -3816,7 +3823,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
@@ -3824,88 +3831,88 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="46"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="51"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="38"/>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="46"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="51"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="39"/>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="46"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="45" t="s">
+      <c r="D46" s="51"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="46"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="45" t="s">
+      <c r="D47" s="51"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="46"/>
+      <c r="D48" s="51"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="45" t="s">
+      <c r="C49" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="46"/>
+      <c r="D49" s="51"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="46"/>
+      <c r="D50" s="51"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="46"/>
+      <c r="D51" s="51"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="46"/>
+      <c r="D52" s="51"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D53" s="46"/>
+      <c r="D53" s="51"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="45" t="s">
+      <c r="C54" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="46"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="46"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="45" t="s">
+      <c r="C56" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="46"/>
+      <c r="D56" s="51"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="41" t="s">
@@ -3937,7 +3944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" s="41" t="s">
         <v>95</v>
       </c>
@@ -3945,7 +3952,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" s="41" t="s">
         <v>96</v>
       </c>
@@ -3953,7 +3960,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B69" s="41" t="s">
         <v>98</v>
       </c>
@@ -3961,7 +3968,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="2:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B71" s="41" t="s">
         <v>100</v>
       </c>
@@ -3969,7 +3976,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="64"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>88</v>
       </c>
@@ -3977,7 +3990,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
         <v>89</v>
       </c>
@@ -3989,78 +4002,78 @@
       <c r="B81" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D81" s="46"/>
+      <c r="D81" s="51"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="38"/>
-      <c r="C82" s="45" t="s">
+      <c r="C82" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D82" s="46"/>
+      <c r="D82" s="51"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="39"/>
-      <c r="C83" s="45" t="s">
+      <c r="C83" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="46"/>
+      <c r="D83" s="51"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C84" s="45" t="s">
+      <c r="C84" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D84" s="46"/>
+      <c r="D84" s="51"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C85" s="45" t="s">
+      <c r="C85" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D85" s="46"/>
+      <c r="D85" s="51"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C86" s="45" t="s">
+      <c r="C86" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D86" s="46"/>
+      <c r="D86" s="51"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C87" s="45" t="s">
+      <c r="C87" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D87" s="46"/>
+      <c r="D87" s="51"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C88" s="45" t="s">
+      <c r="C88" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="46"/>
+      <c r="D88" s="51"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C89" s="45" t="s">
+      <c r="C89" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D89" s="46"/>
+      <c r="D89" s="51"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C90" s="45" t="s">
+      <c r="C90" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="D90" s="46"/>
+      <c r="D90" s="51"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C91" s="45" t="s">
+      <c r="C91" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D91" s="46"/>
+      <c r="D91" s="51"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C92" s="45" t="s">
+      <c r="C92" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D92" s="46"/>
+      <c r="D92" s="51"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="41" t="s">
@@ -4124,6 +4137,34 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C91:D91"/>
@@ -4134,34 +4175,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>